<commit_message>
Submission FR 11 nov
New submission
</commit_message>
<xml_diff>
--- a/Sudan-master/figs/results_table.xlsx
+++ b/Sudan-master/figs/results_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriko/Documents/GitHub/Sudan2019/Sudan-master/figs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriko/GitHub/Sudan2019/Sudan-master/figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3C7E0E65-D2EF-6546-974D-40BA47483A4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60898B56-AEE6-F240-846B-F485536AE7A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1580" windowWidth="23720" windowHeight="14340" activeTab="1"/>
+    <workbookView xWindow="3040" yWindow="1580" windowWidth="23720" windowHeight="14340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results_table" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -650,6 +650,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -657,15 +666,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1022,14 +1022,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F8"/>
+      <selection activeCell="C1" sqref="C1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="12" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -1101,7 +1104,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="L2">
-        <v>9.9000000000000005E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1139,7 +1142,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="L3">
-        <v>8.2000000000000003E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1177,7 +1180,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="L4">
-        <v>9.8000000000000004E-2</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1215,7 +1218,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="L5">
-        <v>9.2999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1253,7 +1256,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="L6">
-        <v>8.2000000000000003E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1291,7 +1294,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="L7">
-        <v>6.6000000000000003E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1329,7 +1332,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="L8">
-        <v>6.3E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1338,11 +1341,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:P1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1354,23 +1357,23 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="5"/>
       <c r="K2" s="1" t="s">
         <v>9</v>
@@ -1380,7 +1383,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
@@ -1413,224 +1416,224 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="10">
         <v>0.11700000000000001</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="10">
         <v>1.639</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10">
         <v>0.06</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <v>0.67500000000000004</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="13">
+      <c r="H4" s="10">
         <v>3.8250000000000002</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="10">
         <v>3.9329999999999998</v>
       </c>
       <c r="J4" s="9"/>
-      <c r="K4" s="14">
+      <c r="K4" s="11">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="L4" s="14">
-        <v>9.9000000000000005E-2</v>
+      <c r="L4" s="11">
+        <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="10">
         <v>0.14899999999999999</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="10">
         <v>1.1759999999999999</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13">
+      <c r="D5" s="10"/>
+      <c r="E5" s="10">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="10">
         <v>1.3660000000000001</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="13">
+      <c r="H5" s="10">
         <v>3.8149999999999999</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="10">
         <v>3.891</v>
       </c>
       <c r="J5" s="9"/>
-      <c r="K5" s="14">
+      <c r="K5" s="11">
         <v>1.2E-2</v>
       </c>
-      <c r="L5" s="14">
-        <v>8.2000000000000003E-2</v>
+      <c r="L5" s="11">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="10">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="10">
         <v>0.309</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="10">
         <v>0.26800000000000002</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="13">
+      <c r="H6" s="10">
         <v>3.8439999999999999</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="10">
         <v>4.1399999999999997</v>
       </c>
       <c r="J6" s="9"/>
-      <c r="K6" s="14">
+      <c r="K6" s="11">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="L6" s="14">
-        <v>9.8000000000000004E-2</v>
+      <c r="L6" s="11">
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="10">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="10">
         <v>0.69799999999999995</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13">
+      <c r="D7" s="10"/>
+      <c r="E7" s="10">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="10">
         <v>1.0009999999999999</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="13">
+      <c r="H7" s="10">
         <v>3.7650000000000001</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="10">
         <v>4.2839999999999998</v>
       </c>
       <c r="J7" s="9"/>
-      <c r="K7" s="14">
+      <c r="K7" s="11">
         <v>2.4E-2</v>
       </c>
-      <c r="L7" s="14">
-        <v>9.2999999999999999E-2</v>
+      <c r="L7" s="11">
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="10">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="10">
         <v>0.72599999999999998</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10">
         <v>0.09</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="10">
         <v>1.2370000000000001</v>
       </c>
       <c r="G8" s="9"/>
-      <c r="H8" s="13">
+      <c r="H8" s="10">
         <v>3.7970000000000002</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="10">
         <v>3.8530000000000002</v>
       </c>
       <c r="J8" s="9"/>
-      <c r="K8" s="14">
+      <c r="K8" s="11">
         <v>1.4E-2</v>
       </c>
-      <c r="L8" s="14">
-        <v>8.2000000000000003E-2</v>
+      <c r="L8" s="11">
+        <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="10">
         <v>0.13500000000000001</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="10">
         <v>0.27</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="10">
         <v>0.76800000000000002</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="13">
+      <c r="H9" s="10">
         <v>3.762</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="10">
         <v>3.927</v>
       </c>
       <c r="J9" s="9"/>
-      <c r="K9" s="14">
+      <c r="K9" s="11">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="L9" s="14">
-        <v>6.6000000000000003E-2</v>
+      <c r="L9" s="11">
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>7</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>0.68300000000000005</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="12">
         <v>1.2350000000000001</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15">
+      <c r="G10" s="12"/>
+      <c r="H10" s="12">
         <v>3.8279999999999998</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="12">
         <v>3.6120000000000001</v>
       </c>
-      <c r="J10" s="15"/>
+      <c r="J10" s="12"/>
       <c r="K10" s="8">
         <v>1.4E-2</v>
       </c>
       <c r="L10" s="8">
-        <v>6.3E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>